<commit_message>
Rettet UTD05 til at bruge workoutplanList.
</commit_message>
<xml_diff>
--- a/05 Test/UTD05 showWorkoutplan.xlsx
+++ b/05 Test/UTD05 showWorkoutplan.xlsx
@@ -37,10 +37,10 @@
     <t xml:space="preserve">TC1</t>
   </si>
   <si>
-    <t xml:space="preserve">Ny Workoutplanlist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">workoutplans.size = 0</t>
+    <t xml:space="preserve">Ny workoutplanList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">workoutplanList.size = 0</t>
   </si>
   <si>
     <t xml:space="preserve">patient = Tom Jensen</t>
@@ -52,13 +52,49 @@
     <t xml:space="preserve">workoutplan:</t>
   </si>
   <si>
-    <t xml:space="preserve">workoutplans.size = 1</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">workoutplanList</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.size = 1</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">workoutplan.title = "Ben"</t>
   </si>
   <si>
-    <t xml:space="preserve">workoutplanlist.addWorkoutplan(workoutplan, patient)</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">workoutplanList</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.addWorkoutplan(workoutplan, patient)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">TC3</t>
@@ -70,7 +106,7 @@
     <t xml:space="preserve">WorkoutplanIsNullException</t>
   </si>
   <si>
-    <t xml:space="preserve">workoutplanlist.addWorkoutplan(besked, patient)</t>
+    <t xml:space="preserve">workoutplanList.addWorkoutplan(besked, patient)</t>
   </si>
   <si>
     <t xml:space="preserve">TC4</t>
@@ -98,7 +134,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">workoutplans</t>
+      <t xml:space="preserve">workoutplanList</t>
     </r>
     <r>
       <rPr>
@@ -119,7 +155,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">workoutplans</t>
+      <t xml:space="preserve">workoutplanList</t>
     </r>
     <r>
       <rPr>
@@ -133,7 +169,25 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">workoutplans[1].title = ”Højre arm”</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">workoutplanList</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[1].title = ”Højre arm”</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">workoutplan.title = "Højre arm"</t>
@@ -264,7 +318,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -281,11 +335,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -374,10 +432,10 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.96"/>
@@ -420,14 +478,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -440,12 +498,12 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4" t="s">
+    <row r="8" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -487,12 +545,12 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="4" t="s">
+    <row r="15" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -503,7 +561,7 @@
       <c r="B16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -511,15 +569,15 @@
       <c r="B17" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="4" t="s">
+    <row r="18" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="7" t="s">
         <v>25</v>
       </c>
     </row>
@@ -528,13 +586,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="4" t="s">
+    <row r="20" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -543,16 +601,16 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="4" t="s">
+    <row r="23" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="4"/>
+      <c r="B24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="4"/>
+      <c r="B25" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>